<commit_message>
new experiments without bug
</commit_message>
<xml_diff>
--- a/Data/Excels/Synthetic/Resumes/Experiment 1.xlsx
+++ b/Data/Excels/Synthetic/Resumes/Experiment 1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -516,31 +516,31 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>-6.53</v>
+        <v>-9.84</v>
       </c>
       <c r="F2" t="n">
-        <v>83.06</v>
+        <v>72.54000000000001</v>
       </c>
       <c r="G2" t="n">
-        <v>77.97</v>
+        <v>66.08</v>
       </c>
       <c r="H2" t="n">
-        <v>3.09</v>
+        <v>14.59</v>
       </c>
       <c r="I2" t="n">
-        <v>82.78</v>
+        <v>62.71</v>
       </c>
       <c r="J2" t="n">
-        <v>85.31999999999999</v>
+        <v>73.42</v>
       </c>
       <c r="K2" t="n">
-        <v>-4.06</v>
+        <v>-10.78</v>
       </c>
       <c r="L2" t="n">
-        <v>89.84</v>
+        <v>83.59</v>
       </c>
       <c r="M2" t="n">
-        <v>86.33</v>
+        <v>75.44</v>
       </c>
     </row>
     <row r="3">
@@ -559,31 +559,31 @@
         <v>2.5</v>
       </c>
       <c r="E3" t="n">
-        <v>13.59</v>
+        <v>13.07</v>
       </c>
       <c r="F3" t="n">
-        <v>52.35</v>
+        <v>57.28</v>
       </c>
       <c r="G3" t="n">
-        <v>60.4</v>
+        <v>66</v>
       </c>
       <c r="H3" t="n">
-        <v>18.23</v>
+        <v>13.57</v>
       </c>
       <c r="I3" t="n">
-        <v>53.73</v>
+        <v>60.38</v>
       </c>
       <c r="J3" t="n">
-        <v>65.59999999999999</v>
+        <v>70</v>
       </c>
       <c r="K3" t="n">
-        <v>26.51</v>
+        <v>24.93</v>
       </c>
       <c r="L3" t="n">
-        <v>51.95</v>
+        <v>58.94</v>
       </c>
       <c r="M3" t="n">
-        <v>70.8</v>
+        <v>78.40000000000001</v>
       </c>
     </row>
     <row r="4">
@@ -602,31 +602,31 @@
         <v>2.5</v>
       </c>
       <c r="E4" t="n">
-        <v>0.73</v>
+        <v>10.7</v>
       </c>
       <c r="F4" t="n">
-        <v>66.56999999999999</v>
+        <v>54.19</v>
       </c>
       <c r="G4" t="n">
-        <v>67.02</v>
+        <v>60.68</v>
       </c>
       <c r="H4" t="n">
-        <v>9.039999999999999</v>
+        <v>20.97</v>
       </c>
       <c r="I4" t="n">
-        <v>67.18000000000001</v>
+        <v>53.27</v>
       </c>
       <c r="J4" t="n">
-        <v>73.78</v>
+        <v>67.44</v>
       </c>
       <c r="K4" t="n">
-        <v>10.77</v>
+        <v>20.7</v>
       </c>
       <c r="L4" t="n">
-        <v>67.42</v>
+        <v>56.38</v>
       </c>
       <c r="M4" t="n">
-        <v>75.48</v>
+        <v>71.04000000000001</v>
       </c>
     </row>
     <row r="5">
@@ -645,31 +645,31 @@
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>-26.59</v>
+        <v>-3.51</v>
       </c>
       <c r="F5" t="n">
-        <v>96.47</v>
+        <v>60.67</v>
       </c>
       <c r="G5" t="n">
-        <v>76.26000000000001</v>
+        <v>58.63</v>
       </c>
       <c r="H5" t="n">
-        <v>-12.81</v>
+        <v>8.17</v>
       </c>
       <c r="I5" t="n">
-        <v>96.78</v>
+        <v>63.41</v>
       </c>
       <c r="J5" t="n">
-        <v>85.79000000000001</v>
+        <v>69.09999999999999</v>
       </c>
       <c r="K5" t="n">
-        <v>-23.84</v>
+        <v>-3.31</v>
       </c>
       <c r="L5" t="n">
-        <v>106.61</v>
+        <v>71.81999999999999</v>
       </c>
       <c r="M5" t="n">
-        <v>86.11</v>
+        <v>69.53</v>
       </c>
     </row>
     <row r="6">
@@ -688,31 +688,31 @@
         <v>10</v>
       </c>
       <c r="E6" t="n">
-        <v>15.39</v>
+        <v>9.65</v>
       </c>
       <c r="F6" t="n">
-        <v>39.35</v>
+        <v>43.94</v>
       </c>
       <c r="G6" t="n">
-        <v>46.5</v>
+        <v>48.6</v>
       </c>
       <c r="H6" t="n">
-        <v>26</v>
+        <v>20.67</v>
       </c>
       <c r="I6" t="n">
-        <v>41.22</v>
+        <v>47.37</v>
       </c>
       <c r="J6" t="n">
-        <v>55.7</v>
+        <v>59.7</v>
       </c>
       <c r="K6" t="n">
-        <v>40.39</v>
+        <v>39.16</v>
       </c>
       <c r="L6" t="n">
-        <v>33.5</v>
+        <v>36.94</v>
       </c>
       <c r="M6" t="n">
-        <v>56.2</v>
+        <v>60.7</v>
       </c>
     </row>
     <row r="7">
@@ -731,31 +731,31 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>-14.56</v>
+        <v>21.5</v>
       </c>
       <c r="F7" t="n">
-        <v>77.20999999999999</v>
+        <v>44.18</v>
       </c>
       <c r="G7" t="n">
-        <v>67.40000000000001</v>
+        <v>56.27</v>
       </c>
       <c r="H7" t="n">
-        <v>2.58</v>
+        <v>18.48</v>
       </c>
       <c r="I7" t="n">
-        <v>74.23</v>
+        <v>54.27</v>
       </c>
       <c r="J7" t="n">
-        <v>76.23</v>
+        <v>66.56</v>
       </c>
       <c r="K7" t="n">
-        <v>-54.29</v>
+        <v>67.77</v>
       </c>
       <c r="L7" t="n">
-        <v>117.71</v>
+        <v>21.54</v>
       </c>
       <c r="M7" t="n">
-        <v>76.28</v>
+        <v>66.81999999999999</v>
       </c>
     </row>
     <row r="8">
@@ -774,31 +774,31 @@
         <v>2.5</v>
       </c>
       <c r="E8" t="n">
-        <v>17.15</v>
+        <v>30.13</v>
       </c>
       <c r="F8" t="n">
-        <v>44.34</v>
+        <v>41.33</v>
       </c>
       <c r="G8" t="n">
-        <v>53.4</v>
+        <v>59.26</v>
       </c>
       <c r="H8" t="n">
-        <v>26.33</v>
+        <v>11.99</v>
       </c>
       <c r="I8" t="n">
-        <v>46.18</v>
+        <v>59.64</v>
       </c>
       <c r="J8" t="n">
-        <v>62.65</v>
+        <v>67.59</v>
       </c>
       <c r="K8" t="n">
-        <v>38.91</v>
+        <v>43.85</v>
       </c>
       <c r="L8" t="n">
-        <v>40.75</v>
+        <v>41.79</v>
       </c>
       <c r="M8" t="n">
-        <v>66.67</v>
+        <v>74.38</v>
       </c>
     </row>
     <row r="9">
@@ -817,31 +817,31 @@
         <v>2.5</v>
       </c>
       <c r="E9" t="n">
-        <v>-1.57</v>
+        <v>3.46</v>
       </c>
       <c r="F9" t="n">
-        <v>68.16</v>
+        <v>57.01</v>
       </c>
       <c r="G9" t="n">
-        <v>66.98</v>
+        <v>58.96</v>
       </c>
       <c r="H9" t="n">
-        <v>9.279999999999999</v>
+        <v>17.56</v>
       </c>
       <c r="I9" t="n">
-        <v>68.3</v>
+        <v>55.51</v>
       </c>
       <c r="J9" t="n">
-        <v>75.19</v>
+        <v>67.34999999999999</v>
       </c>
       <c r="K9" t="n">
-        <v>9.99</v>
+        <v>28.84</v>
       </c>
       <c r="L9" t="n">
-        <v>68.54000000000001</v>
+        <v>48.99</v>
       </c>
       <c r="M9" t="n">
-        <v>76.12</v>
+        <v>68.84</v>
       </c>
     </row>
     <row r="10">
@@ -860,31 +860,31 @@
         <v>10</v>
       </c>
       <c r="E10" t="n">
-        <v>49.28</v>
+        <v>56.55</v>
       </c>
       <c r="F10" t="n">
-        <v>22.26</v>
+        <v>20.36</v>
       </c>
       <c r="G10" t="n">
-        <v>43.87</v>
+        <v>46.91</v>
       </c>
       <c r="H10" t="n">
-        <v>62.38</v>
+        <v>75.31</v>
       </c>
       <c r="I10" t="n">
-        <v>20.78</v>
+        <v>14.69</v>
       </c>
       <c r="J10" t="n">
-        <v>55.27</v>
+        <v>59.54</v>
       </c>
       <c r="K10" t="n">
-        <v>55.77</v>
+        <v>76.03</v>
       </c>
       <c r="L10" t="n">
-        <v>24.61</v>
+        <v>14.59</v>
       </c>
       <c r="M10" t="n">
-        <v>55.65</v>
+        <v>60.87</v>
       </c>
     </row>
     <row r="11">
@@ -903,31 +903,461 @@
         <v>10</v>
       </c>
       <c r="E11" t="n">
-        <v>-25.15</v>
+        <v>-16.74</v>
       </c>
       <c r="F11" t="n">
-        <v>80.73999999999999</v>
+        <v>62.08</v>
       </c>
       <c r="G11" t="n">
-        <v>64.52</v>
+        <v>53.16</v>
       </c>
       <c r="H11" t="n">
-        <v>-7.6</v>
+        <v>22.82</v>
       </c>
       <c r="I11" t="n">
-        <v>81.23999999999999</v>
+        <v>50.65</v>
       </c>
       <c r="J11" t="n">
-        <v>75.48</v>
+        <v>65.59999999999999</v>
       </c>
       <c r="K11" t="n">
-        <v>-42.56</v>
+        <v>24.36</v>
       </c>
       <c r="L11" t="n">
-        <v>107.32</v>
+        <v>49.71</v>
       </c>
       <c r="M11" t="n">
-        <v>75.27</v>
+        <v>65.70999999999999</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>4.06</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Planar</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>1.31</v>
+      </c>
+      <c r="F12" t="n">
+        <v>378.98</v>
+      </c>
+      <c r="G12" t="n">
+        <v>383.74</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="I12" t="n">
+        <v>378.35</v>
+      </c>
+      <c r="J12" t="n">
+        <v>378.33</v>
+      </c>
+      <c r="K12" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="L12" t="n">
+        <v>379.13</v>
+      </c>
+      <c r="M12" t="n">
+        <v>404.43</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Planar</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="E13" t="n">
+        <v>2.65</v>
+      </c>
+      <c r="F13" t="n">
+        <v>604.8200000000001</v>
+      </c>
+      <c r="G13" t="n">
+        <v>621.2</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="I13" t="n">
+        <v>610.28</v>
+      </c>
+      <c r="J13" t="n">
+        <v>610.8</v>
+      </c>
+      <c r="K13" t="n">
+        <v>62.2</v>
+      </c>
+      <c r="L13" t="n">
+        <v>247.01</v>
+      </c>
+      <c r="M13" t="n">
+        <v>653.6</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>4.55</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Planar</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D14" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="E14" t="n">
+        <v>64.84999999999999</v>
+      </c>
+      <c r="F14" t="n">
+        <v>134.41</v>
+      </c>
+      <c r="G14" t="n">
+        <v>381.98</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="I14" t="n">
+        <v>377.9</v>
+      </c>
+      <c r="J14" t="n">
+        <v>378.02</v>
+      </c>
+      <c r="K14" t="n">
+        <v>64.62</v>
+      </c>
+      <c r="L14" t="n">
+        <v>141.95</v>
+      </c>
+      <c r="M14" t="n">
+        <v>400.88</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>15.37</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Planar</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>10</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" t="n">
+        <v>72.06</v>
+      </c>
+      <c r="F15" t="n">
+        <v>61.57</v>
+      </c>
+      <c r="G15" t="n">
+        <v>220.36</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="I15" t="n">
+        <v>222.22</v>
+      </c>
+      <c r="J15" t="n">
+        <v>222.45</v>
+      </c>
+      <c r="K15" t="n">
+        <v>65.75</v>
+      </c>
+      <c r="L15" t="n">
+        <v>77.68000000000001</v>
+      </c>
+      <c r="M15" t="n">
+        <v>226.81</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>10</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Planar</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" t="n">
+        <v>10</v>
+      </c>
+      <c r="E16" t="n">
+        <v>28.95</v>
+      </c>
+      <c r="F16" t="n">
+        <v>133.22</v>
+      </c>
+      <c r="G16" t="n">
+        <v>187.5</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="I16" t="n">
+        <v>186.84</v>
+      </c>
+      <c r="J16" t="n">
+        <v>188.5</v>
+      </c>
+      <c r="K16" t="n">
+        <v>32.96</v>
+      </c>
+      <c r="L16" t="n">
+        <v>132.33</v>
+      </c>
+      <c r="M16" t="n">
+        <v>197.4</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>19.26</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Planar</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>10</v>
+      </c>
+      <c r="D17" t="n">
+        <v>10</v>
+      </c>
+      <c r="E17" t="n">
+        <v>-0.57</v>
+      </c>
+      <c r="F17" t="n">
+        <v>196.52</v>
+      </c>
+      <c r="G17" t="n">
+        <v>195.38</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="I17" t="n">
+        <v>197.88</v>
+      </c>
+      <c r="J17" t="n">
+        <v>198.23</v>
+      </c>
+      <c r="K17" t="n">
+        <v>55.49</v>
+      </c>
+      <c r="L17" t="n">
+        <v>89.43000000000001</v>
+      </c>
+      <c r="M17" t="n">
+        <v>200.88</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>45.63</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Gradual</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="E18" t="n">
+        <v>43.8</v>
+      </c>
+      <c r="F18" t="n">
+        <v>84.73</v>
+      </c>
+      <c r="G18" t="n">
+        <v>150.76</v>
+      </c>
+      <c r="H18" t="n">
+        <v>2.99</v>
+      </c>
+      <c r="I18" t="n">
+        <v>152.42</v>
+      </c>
+      <c r="J18" t="n">
+        <v>157.11</v>
+      </c>
+      <c r="K18" t="n">
+        <v>45.99</v>
+      </c>
+      <c r="L18" t="n">
+        <v>85.03</v>
+      </c>
+      <c r="M18" t="n">
+        <v>157.44</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>43.22</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Gradual</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D19" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="E19" t="n">
+        <v>35.4</v>
+      </c>
+      <c r="F19" t="n">
+        <v>106.43</v>
+      </c>
+      <c r="G19" t="n">
+        <v>164.74</v>
+      </c>
+      <c r="H19" t="n">
+        <v>1.47</v>
+      </c>
+      <c r="I19" t="n">
+        <v>167.13</v>
+      </c>
+      <c r="J19" t="n">
+        <v>169.6</v>
+      </c>
+      <c r="K19" t="n">
+        <v>37.64</v>
+      </c>
+      <c r="L19" t="n">
+        <v>106.63</v>
+      </c>
+      <c r="M19" t="n">
+        <v>170.99</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>81</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Gradual</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" t="n">
+        <v>10</v>
+      </c>
+      <c r="E20" t="n">
+        <v>37.94</v>
+      </c>
+      <c r="F20" t="n">
+        <v>77.79000000000001</v>
+      </c>
+      <c r="G20" t="n">
+        <v>125.33</v>
+      </c>
+      <c r="H20" t="n">
+        <v>42.09</v>
+      </c>
+      <c r="I20" t="n">
+        <v>77.56</v>
+      </c>
+      <c r="J20" t="n">
+        <v>133.94</v>
+      </c>
+      <c r="K20" t="n">
+        <v>4.69</v>
+      </c>
+      <c r="L20" t="n">
+        <v>127.79</v>
+      </c>
+      <c r="M20" t="n">
+        <v>134.07</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>85.86</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Gradual</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>10</v>
+      </c>
+      <c r="D21" t="n">
+        <v>10</v>
+      </c>
+      <c r="E21" t="n">
+        <v>57.95</v>
+      </c>
+      <c r="F21" t="n">
+        <v>53.95</v>
+      </c>
+      <c r="G21" t="n">
+        <v>128.3</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="I21" t="n">
+        <v>135.66</v>
+      </c>
+      <c r="J21" t="n">
+        <v>137.03</v>
+      </c>
+      <c r="K21" t="n">
+        <v>3.12</v>
+      </c>
+      <c r="L21" t="n">
+        <v>133.4</v>
+      </c>
+      <c r="M21" t="n">
+        <v>137.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>